<commit_message>
solve cp prac constructive problems
</commit_message>
<xml_diff>
--- a/Cp Prac/Cp Pep Sheet/All Combine.xlsx
+++ b/Cp Prac/Cp Pep Sheet/All Combine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\Cp Prac\Cp Pep Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4310B7-5766-44C1-92FB-AF0F23E21FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619E6C22-8451-4210-B099-34CC04249BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2460" windowWidth="19200" windowHeight="7575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary Lifting" sheetId="1" r:id="rId1"/>
@@ -2128,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E76437-F032-4C72-8139-803DC81A3669}">
   <dimension ref="A3:J301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2338,7 +2338,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="I12" t="s">
         <v>18</v>
@@ -2386,7 +2386,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
rename file and del
</commit_message>
<xml_diff>
--- a/Cp Prac/Cp Pep Sheet/All Combine.xlsx
+++ b/Cp Prac/Cp Pep Sheet/All Combine.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\Cp Prac\Cp Pep Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5B2969-4885-447C-BCC3-FC765270E05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36024B8-4634-4D30-ACDD-B3DF0ECCA2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2137,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E76437-F032-4C72-8139-803DC81A3669}">
   <dimension ref="A3:J301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C199" sqref="C199"/>
+    <sheetView tabSelected="1" topLeftCell="C154" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C171" sqref="C171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5245,7 +5245,7 @@
         <v>14</v>
       </c>
       <c r="E143" s="5" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="I143" t="s">
         <v>251</v>
@@ -5533,7 +5533,7 @@
         <v>14</v>
       </c>
       <c r="E155" s="5" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="I155" t="s">
         <v>275</v>
@@ -5773,7 +5773,7 @@
         <v>14</v>
       </c>
       <c r="E165" s="5" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="I165" t="s">
         <v>295</v>
@@ -5869,7 +5869,7 @@
         <v>14</v>
       </c>
       <c r="E169" s="5" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="I169" t="s">
         <v>303</v>
@@ -5893,7 +5893,7 @@
         <v>14</v>
       </c>
       <c r="E170" s="5" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="I170" t="s">
         <v>305</v>
@@ -6445,7 +6445,7 @@
         <v>14</v>
       </c>
       <c r="E193" s="5" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="I193" t="s">
         <v>349</v>

</xml_diff>